<commit_message>
Day12- Happy New Year
</commit_message>
<xml_diff>
--- a/src/test/java/resources/Capitals.xlsx
+++ b/src/test/java/resources/Capitals.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechPro\Desktop\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -87,12 +87,25 @@
   </si>
   <si>
     <t>Oslo</t>
+  </si>
+  <si>
+    <t>POPULATION</t>
+  </si>
+  <si>
+    <t>150000</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>54000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -354,7 +367,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
@@ -369,6 +382,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -377,6 +393,9 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s" s="0">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -385,6 +404,9 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s" s="0">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -392,6 +414,9 @@
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>